<commit_message>
Added Income project(in processing). Added V3 in Software developer in Azerbaijan(in processing)
</commit_message>
<xml_diff>
--- a/Flags/V1/added new data.xlsx
+++ b/Flags/V1/added new data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Analyst\Flags\V1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Data Analyst\Flags\V1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF408AF4-A313-450A-8D79-2B6ABA003F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A9833CA-3371-4F00-A0BF-14103C5744E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="317">
   <si>
     <t>name</t>
   </si>
@@ -964,6 +964,24 @@
   </si>
   <si>
     <t>Germany</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/5/56/Flag_of_Haiti.svg/1920px-Flag_of_Haiti.svg.png</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/8/82/Flag_of_Honduras.svg/1920px-Flag_of_Honduras.svg.png</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/5/5b/Flag_of_Hong_Kong.svg/1280px-Flag_of_Hong_Kong.svg.png</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/c/c1/Flag_of_Hungary.svg/1920px-Flag_of_Hungary.svg.png</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/c/ce/Flag_of_Iceland.svg/1280px-Flag_of_Iceland.svg.png</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/en/thumb/4/41/Flag_of_India.svg/1280px-Flag_of_India.svg.png</t>
   </si>
 </sst>
 </file>
@@ -1862,8 +1880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" topLeftCell="A163" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8576,6 +8594,9 @@
       <c r="B67" t="s">
         <v>160</v>
       </c>
+      <c r="C67" s="1">
+        <v>2</v>
+      </c>
       <c r="D67" s="1">
         <v>4</v>
       </c>
@@ -8674,6 +8695,9 @@
       <c r="B68" t="s">
         <v>162</v>
       </c>
+      <c r="C68" s="1">
+        <v>2</v>
+      </c>
       <c r="D68" s="1">
         <v>3</v>
       </c>
@@ -8772,6 +8796,9 @@
       <c r="B69" t="s">
         <v>164</v>
       </c>
+      <c r="C69" s="1">
+        <v>2</v>
+      </c>
       <c r="D69" s="1">
         <v>3</v>
       </c>
@@ -8870,6 +8897,9 @@
       <c r="B70" t="s">
         <v>166</v>
       </c>
+      <c r="C70" s="1">
+        <v>1</v>
+      </c>
       <c r="D70" s="1">
         <v>1</v>
       </c>
@@ -9553,6 +9583,12 @@
       <c r="A77" t="s">
         <v>179</v>
       </c>
+      <c r="B77" t="s">
+        <v>311</v>
+      </c>
+      <c r="C77" s="1">
+        <v>5</v>
+      </c>
       <c r="D77" s="1">
         <v>1</v>
       </c>
@@ -9648,6 +9684,12 @@
       <c r="A78" t="s">
         <v>180</v>
       </c>
+      <c r="B78" t="s">
+        <v>312</v>
+      </c>
+      <c r="C78" s="1">
+        <v>4</v>
+      </c>
       <c r="D78" s="1">
         <v>1</v>
       </c>
@@ -9743,6 +9785,12 @@
       <c r="A79" t="s">
         <v>181</v>
       </c>
+      <c r="B79" t="s">
+        <v>313</v>
+      </c>
+      <c r="C79" s="1">
+        <v>1</v>
+      </c>
       <c r="D79" s="1">
         <v>5</v>
       </c>
@@ -9838,6 +9886,12 @@
       <c r="A80" t="s">
         <v>182</v>
       </c>
+      <c r="B80" t="s">
+        <v>314</v>
+      </c>
+      <c r="C80" s="1">
+        <v>1</v>
+      </c>
       <c r="D80" s="1">
         <v>3</v>
       </c>
@@ -9933,6 +9987,12 @@
       <c r="A81" t="s">
         <v>183</v>
       </c>
+      <c r="B81" t="s">
+        <v>315</v>
+      </c>
+      <c r="C81" s="1">
+        <v>2</v>
+      </c>
       <c r="D81" s="1">
         <v>3</v>
       </c>
@@ -10027,6 +10087,12 @@
     <row r="82" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>184</v>
+      </c>
+      <c r="B82" t="s">
+        <v>316</v>
+      </c>
+      <c r="C82" s="1">
+        <v>1</v>
       </c>
       <c r="D82" s="1">
         <v>5</v>

</xml_diff>